<commit_message>
Added input processing into main - 12/12/2025
</commit_message>
<xml_diff>
--- a/Input/Insurance House Fields and files 1.xlsx
+++ b/Input/Insurance House Fields and files 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirmal\Documents\UiPath\UnityBrokers_Dispatcher\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9043FC7-1F84-48DD-A628-98B69C98BDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF36EFA-7A78-416F-974E-AE9B221063CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3D5EF9B-2C89-440C-91A8-5F44550ADBF0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Assured Name</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>21/04/2002</t>
-  </si>
-  <si>
-    <t>ABU DHABI</t>
   </si>
   <si>
     <t>784-1974-7959051-1</t>
@@ -624,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68E5278-26C0-4FF4-A584-CF1A80280783}">
   <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,8 +632,7 @@
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -836,16 +832,16 @@
         <v>49</v>
       </c>
       <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" t="s">
-        <v>58</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
         <v>52</v>
@@ -857,25 +853,28 @@
         <v>56</v>
       </c>
       <c r="AA2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AI2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK2" t="s">
         <v>59</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS2" t="s">
         <v>60</v>
       </c>
-      <c r="AO2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS2" t="s">
+      <c r="AU2" t="s">
         <v>61</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>